<commit_message>
Baltas kastes testēšana un koda kļūdu labojumi
</commit_message>
<xml_diff>
--- a/LVT_TpM_TP_V_1_0_2_.xlsx
+++ b/LVT_TpM_TP_V_1_0_2_.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12900" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12900" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Apraksts" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="182">
   <si>
     <t>Identifikatoru atšifrējjums</t>
   </si>
@@ -258,10 +258,6 @@
     <t>Parādīsies otrais jautājums</t>
   </si>
   <si>
-    <t>1) Nospiest klaviatūras taustiņu ar apzīmējumu "2"
-3) Peles kreisā taustiņa klikšķis uz pogas ar apzīmējumu "OK"</t>
-  </si>
-  <si>
     <t>Pārbauda, kas notiek kad ievada nepareizo atbildi</t>
   </si>
   <si>
@@ -269,10 +265,6 @@
   </si>
   <si>
     <t>TP.TES.AI.03.</t>
-  </si>
-  <si>
-    <t>1) Nospiest klaviatūras taustiņu ar apzīmējumu "a"
-3) Peles kreisā taustiņa klikšķis uz pogas ar apzīmējumu "OK"</t>
   </si>
   <si>
     <t>1) Jābūt startētai programmai "Tests par Mainīgajiem"
@@ -305,9 +297,6 @@
   </si>
   <si>
     <t>PAR</t>
-  </si>
-  <si>
-    <t>Parāda</t>
   </si>
   <si>
     <t>TP.ATB.PAR.01.</t>
@@ -356,57 +345,312 @@
     <t>Parāda, ka jautājumam ir nepareiza atbilde</t>
   </si>
   <si>
-    <t xml:space="preserve">Pārbauda vai lietotājam parādīsies </t>
+    <t>TZ.01.B.</t>
+  </si>
+  <si>
+    <t>Gustavs Narvils</t>
+  </si>
+  <si>
+    <t>Veiksmīgs</t>
+  </si>
+  <si>
+    <t>13.06.2022.</t>
+  </si>
+  <si>
+    <t>TZ.02.B.</t>
+  </si>
+  <si>
+    <t>TZ.03.B.</t>
+  </si>
+  <si>
+    <t>TZ.04.B.</t>
+  </si>
+  <si>
+    <t>TZ.05.B.</t>
+  </si>
+  <si>
+    <t>TZ.06.B.</t>
+  </si>
+  <si>
+    <t>TZ.07.B.</t>
+  </si>
+  <si>
+    <t>TZ.08.B.</t>
+  </si>
+  <si>
+    <t>TZ.09.B.</t>
+  </si>
+  <si>
+    <t>TZ.10.B.</t>
+  </si>
+  <si>
+    <t>TZ.10.W.</t>
+  </si>
+  <si>
+    <t>TZ.01.W.</t>
+  </si>
+  <si>
+    <t>TZ.02.W.</t>
+  </si>
+  <si>
+    <t>TZ.03.W.</t>
+  </si>
+  <si>
+    <t>TZ.04.W.</t>
+  </si>
+  <si>
+    <t>TZ.05.W.</t>
+  </si>
+  <si>
+    <t>TZ.06.W.</t>
+  </si>
+  <si>
+    <t>TZ.07.W.</t>
+  </si>
+  <si>
+    <t>TZ.08.W.</t>
+  </si>
+  <si>
+    <t>TZ.09.W.</t>
+  </si>
+  <si>
+    <t>PR.TES.AI.04.</t>
+  </si>
+  <si>
+    <t>1) Jābūt startētai programmai "Tests par Mainīgajiem"
+2) Jābūt aizvērtam sākuma paziņojuma logam
+3) Lietotājam jātbild uz iepreikšējiem 4 jautājumiem</t>
+  </si>
+  <si>
+    <t>Pārbauda vai var iesniegt pareizo atbildi piektajam jautājumam</t>
+  </si>
+  <si>
+    <t>1) Nospiest klaviatūras taustiņu ar apzīmējumu "3"
+2) Nospiest klaviatūras taustiņu ar apzīmējumu "4"
+3) Peles kreisā taustiņa klikšķis uz pogas ar apzīmējumu "OK"</t>
+  </si>
+  <si>
+    <t>PR.TES.AI.05.</t>
+  </si>
+  <si>
+    <t>1) Jābūt startētai programmai "Tests par Mainīgajiem"
+2) Jābūt aizvērtam sākuma paziņojuma logam
+3) Lietotājam jātbild uz iepreikšējiem 8 jautājumiem</t>
+  </si>
+  <si>
+    <t>Pārbauda vai var iesniegt pareizo atbildi devītajam jautājumam</t>
   </si>
   <si>
     <t>1) Nospiest klaviatūras taustiņu ar apzīmējumu "2"
-2) Peles kreisā taustiņa klikšķis uz pogas ar apzīmējumu "OK"
-3) Lietotājs, katra nākamā atbilžu logā nospiež klaviatūras taustiņu ar apzīmējumu "1"
-4) Un spiež pēc katra ievadītās atbildes ar peles kreiso taustiņa klikšķi nospiež pogu ar apzīmējumu "OK"
-5) Tad, kad tiek beigu logā lietotājs nospiež klaviatūras taustiņu ar apzīmējumu "1".
-6) Peles kreisā taustiņa klikškis uz pogas ar apzīmējumu "OK"</t>
-  </si>
-  <si>
-    <t>Parādīsies pirmā jautājuma atbilžu logs, kura apakšā jābūt rakstītam "Jo tikai Int un Double tipa mainīgos šajā gadijumā var izmantot lai darītu matemātiskās darbības!"</t>
-  </si>
-  <si>
-    <t>TZ.01.B.</t>
-  </si>
-  <si>
-    <t>Gustavs Narvils</t>
-  </si>
-  <si>
-    <t>Veiksmīgs</t>
-  </si>
-  <si>
-    <t>13.06.2022.</t>
-  </si>
-  <si>
-    <t>TZ.02.B.</t>
-  </si>
-  <si>
-    <t>TZ.03.B.</t>
-  </si>
-  <si>
-    <t>TZ.04.B.</t>
-  </si>
-  <si>
-    <t>TZ.05.B.</t>
-  </si>
-  <si>
-    <t>TZ.06.B.</t>
-  </si>
-  <si>
-    <t>TZ.07.B.</t>
-  </si>
-  <si>
-    <t>TZ.08.B.</t>
-  </si>
-  <si>
-    <t>TZ.09.B.</t>
-  </si>
-  <si>
-    <t>TZ.10.B.</t>
+2) Nospiest klaviatūras taustiņu ar apzīmējumu "4"
+3) Peles kreisā taustiņa klikšķis uz pogas ar apzīmējumu "OK"</t>
+  </si>
+  <si>
+    <t>TP.TES.AI.06.</t>
+  </si>
+  <si>
+    <t>TP.TES.AI.07.</t>
+  </si>
+  <si>
+    <t>1) Jābūt startētai programmai "Tests par Mainīgajiem"
+2) Jābūt aizvērtam sākuma paziņojuma logam
+3) Lietotājam jātbild uz iepreikšējiem 2 jautājumiem</t>
+  </si>
+  <si>
+    <t>Pārbauda vai var iesniegt nepareizo atbildi trešajam jautājumam</t>
+  </si>
+  <si>
+    <t>1) Nospiest klaviatūras taustiņu ar apzīmējumu "2"
+2) Peles kreisā taustiņa klikšķis uz pogas ar apzīmējumu "OK"</t>
+  </si>
+  <si>
+    <t>1) Nospiest klaviatūras taustiņu ar apzīmējumu "a"
+2) Peles kreisā taustiņa klikšķis uz pogas ar apzīmējumu "OK"</t>
+  </si>
+  <si>
+    <t>1) Nospiest klaviatūras taustiņu ar apzīmējumu "1"
+2) Nospiest klaviatūras taustiņu ar apzīmējumu "4"
+3) Peles kreisā taustiņa klikšķis uz pogas ar apzīmējumu "OK"</t>
+  </si>
+  <si>
+    <t>1) Jābūt startētai programmai "Tests par Mainīgajiem"
+2) Jābūt aizvērtam sākuma paziņojuma logam
+3) Lietotājam jātbild uz iepreikšējiem 6 jautājumiem</t>
+  </si>
+  <si>
+    <t>Pārbauda vai var iesniegt nepareizo atbildi septītajam jautājumam</t>
+  </si>
+  <si>
+    <t>TP.ATB.PAR.04.</t>
+  </si>
+  <si>
+    <t>TP.TES.AI.08.</t>
+  </si>
+  <si>
+    <t>1) Jābūt startētai programmai "Tests par Mainīgajiem"
+2) Jābūt aizvērtam sākuma paziņojuma logam
+3) Lietotājam jātbild uz iepreikšējiem 7 jautājumiem</t>
+  </si>
+  <si>
+    <t>1) Mainīgajam Pareizi pieskaitas skaitlis 1
+2) Mainīgā Pareizi8 vērtība paliek par true
+3) Mainīgā Atbilde8 vērtība paliek par " - Pareizi!"
+4) Mainīgā atbilde vērtība paliek par 0
+5) Izdara metodi Jautajums10()</t>
+  </si>
+  <si>
+    <t>1) Mainīgajam Pareizi pieskaitas skaitlis 1
+2) Mainīgā Pareizi9 vērtība paliek par true
+3) Mainīgā Atbilde9 vērtība paliek par " - Pareizi!"
+4) Mainīgā atbilde vērtība paliek par 0
+5) Izdara metodi Jautajums10()</t>
+  </si>
+  <si>
+    <t>1) Mainīgajam Pareizi pieskaitas skaitlis 1
+2) Mainīgā Pareizi5 vērtība paliek par true
+3) Mainīgā Atbilde5 vērtība paliek par " - Pareizi!" 
+4) Mainīgā atbilde vērtība paliek par 0
+5) Izdara metodi Jautajums6()</t>
+  </si>
+  <si>
+    <t>Pārbauda vai var iesniegt pareizo atbildi astotajam jautājumam</t>
+  </si>
+  <si>
+    <t>Parāda rezultatu</t>
+  </si>
+  <si>
+    <t>Parāda uz cik jautājumiem ir atbildēts pareizi</t>
+  </si>
+  <si>
+    <t>1) Jābūt startētai programmai "Tests par Mainīgajiem"
+2) Jābūt aizvērtam sākuma paziņojuma logam
+3) Lietotājam jātbild uz visiem 10 jautājumiem nepareizi</t>
+  </si>
+  <si>
+    <t>1) Jābūt startētai programmai "Tests par Mainīgajiem"
+2) Jābūt aizvērtam sākuma paziņojuma logam
+3) Lietotājam jātbild uz visiem iepriekšējiem 8 jautājumiem nepareizi</t>
+  </si>
+  <si>
+    <t>Pārbauda vai programma parāda uz cik daudziem jautājumiem atbildēja pareizi</t>
+  </si>
+  <si>
+    <t>1) Nospiest klaviatūras taustiņu ar apzīmējumu "1"
+2) Nospiest klaviatūras taustiņu ar apzīmējumu "3"
+3) Peles kreisā taustiņa klikšķis uz pogas ar apzīmējumu "OK"
+4) Nospiest klaviatūras taustiņu ar apzīmējumu "1"
+5) Nospiest klaviatūras taustiņu ar apzīmējumu "2"
+6) Nospiest klaviatūras taustiņu ar apzīmējumu "3"
+7) Peles kreisā taustiņa klikšķis uz pogas ar apzīmējumu "OK"</t>
+  </si>
+  <si>
+    <t>PR.ATB.06.</t>
+  </si>
+  <si>
+    <t>1) Mainigajam Pareizi vērtībai jāpieskaitās skaitlis 2
+2) Pareizi9 un Pareizi10 vērtība paliek par true
+3) Atbilde9 un Atbilde10 vērtība paliek par " - Pareizi!"
+4) Mainīga atbilde vērtība paliek par 0
+5) Izdara metodi rezultats()
+6) Beigu logā izdrukājas Pareizi vērtība</t>
+  </si>
+  <si>
+    <t>Neveiksmīgs</t>
+  </si>
+  <si>
+    <t>KZ.ATB.01.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mainīgā atbilde vērtība netika iztukšota tādēļ palika 123 nevis 0 </t>
+  </si>
+  <si>
+    <t>Apskatīt jautājumus</t>
+  </si>
+  <si>
+    <t>TP.ATB.PAR.05.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pārbauda vai var apskatīt iepriekšējos jautājumus </t>
+  </si>
+  <si>
+    <t>1) Nospiest klaviatūras taustiņu ar apzīmējumu "1"
+2) Peles kreisā taustiņa klikšķis uz pogas ar apzīmējumu "OK"</t>
+  </si>
+  <si>
+    <t>1) Mainīgā atbilde vērtība paliek par 0
+2) Izdara metodi Jautajums9()</t>
+  </si>
+  <si>
+    <t>1) Mainīgā atbilde vērtība paliek par 0
+2) Izdara metodi Jautajums4()</t>
+  </si>
+  <si>
+    <t>TP.ATB.PAR.06.</t>
+  </si>
+  <si>
+    <t>TP.ATB.PAR.08.</t>
+  </si>
+  <si>
+    <t>KZ.ATB.02.</t>
+  </si>
+  <si>
+    <t>1) Jābūt startētai programmai "Tests par Mainīgajiem"
+2) Jābūt aizvērtam sākuma paziņojuma logam
+3) Lietotājam jātbild uz visiem iepriekšējiem 9 jautājumiem nepareizi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mainīgā atbilde vērtība netika iztukšota tādēļ palika 13 nevis 0 </t>
+  </si>
+  <si>
+    <t>1) Nospiest klaviatūras taustiņu ar apzīmējumu "1"
+2) Nospiest klaviatūras taustiņu ar apzīmējumu "2"
+3) Nospiest klaviatūras taustiņu ar apzīmējumu "3"
+4) Peles kreisā taustiņa klikšķis uz pogas ar apzīmējumu "OK"</t>
+  </si>
+  <si>
+    <t>1) Mainigajam Pareizi vērtībai jāpieskaitās skaitlis 1
+2) Pareizi10 vērtība paliek par true
+3) Atbilde10 vērtība paliek par " - Pareizi!"
+4) Mainīga atbilde vērtība paliek par 0
+5) Izdara metodi rezultats()
+6) Beigu logā izdrukājas Pareizi vērtība</t>
+  </si>
+  <si>
+    <t>TP.ATB.PAR.07.</t>
+  </si>
+  <si>
+    <t>1) Nospiest klaviatūras taustiņu ar apzīmējumu "7"
+2) Peles kreisā taustiņa klikšķis uz pogas ar apzīmējumu "OK"</t>
+  </si>
+  <si>
+    <t>Apskatīties Jautājumus</t>
+  </si>
+  <si>
+    <t>1) Jābūt startētai programmai "Tests par Mainīgajiem"
+2) Jābūt aizvērtam sākuma paziņojuma logam
+3) Lietotājam jātbild uz visiem 10 jautājumiem pareizi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pārbauda vai var apskatīt iepriekšējos jautājumus un parādīties apakšā skaidrojumam, kāpēc tas bija nepareizs </t>
+  </si>
+  <si>
+    <t>Parādīsies uz ekrāna pirmais jautājums un apakšā būs rakstīts kāpēc man tas bija nepareizs</t>
+  </si>
+  <si>
+    <t>1) Nospiest klaviatūras taustiņu ar apzīmējumu "5"
+2) Peles kreisā taustiņa klikšķis uz pogas ar apzīmējumu "OK"</t>
+  </si>
+  <si>
+    <t>1) Izdara metodi atbilde5()
+2) Pareizi5 vērtībai ir jābūt true, tādēļ izdrukāsies 5. jautājums un parādīsies, ka tas bija pareizs</t>
+  </si>
+  <si>
+    <t>1) Izdara metodi atbilde7()
+2) Pareizi7 vērtībai ir jābūt false, tādēļ izdrukāsies 7. jautājums un parādīsies, ka tas bija nepareizs</t>
+  </si>
+  <si>
+    <t>1) Izdara metodi atbilde1()
+2) Pareizi1 vērtībai ir jābūt false, tādēļ izdrukāsies 1. jautājums un parādīsies, ka tas bija nepareizs</t>
   </si>
 </sst>
 </file>
@@ -495,7 +739,7 @@
       <charset val="186"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,6 +770,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -539,7 +789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -557,6 +807,16 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -579,14 +839,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -872,7 +1125,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B19"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,28 +1134,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -925,12 +1178,12 @@
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -958,10 +1211,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -982,10 +1235,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>90</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1001,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,7 +1266,7 @@
     <col min="2" max="2" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1021,11 +1274,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -1033,13 +1286,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="13"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -1047,7 +1300,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -1055,7 +1308,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>42</v>
       </c>
@@ -1063,55 +1316,64 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1124,22 +1386,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="46.85546875" customWidth="1"/>
     <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="63.5703125" customWidth="1"/>
     <col min="6" max="6" width="26.85546875" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1170,431 +1432,612 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="17" t="s">
+      <c r="E16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="H8" s="16" t="s">
+      <c r="G16" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="16" t="s">
+    <row r="19" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="C21" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="H9" s="16" t="s">
+      <c r="G21" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="H21" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="16" t="s">
+    <row r="22" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="17" t="s">
+      <c r="C22" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="H10" s="16" t="s">
+      <c r="G22" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="H22" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-    </row>
-    <row r="12" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="F12" s="17" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+    </row>
+    <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="E13" s="16" t="s">
+      <c r="G24" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="C25" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="F14" s="17" t="s">
+      <c r="G25" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G14" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="H14" s="16" t="s">
+      <c r="G26" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="H26" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-    </row>
-    <row r="16" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="17" t="s">
+    <row r="27" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F27" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G16" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="H16" s="16" t="s">
+      <c r="G27" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="H27" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
+    <row r="28" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A23:H23"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A4:H4"/>
@@ -1609,11 +2052,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,10 +2064,10 @@
     <col min="1" max="1" width="29.85546875" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="49.140625" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1655,391 +2098,546 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>107</v>
+      <c r="A3" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="E3" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>111</v>
+      <c r="A5" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>109</v>
+      <c r="E5" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>112</v>
+      <c r="A6" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>109</v>
+      <c r="E6" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>113</v>
+      <c r="A8" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>109</v>
+      <c r="E8" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>114</v>
+      <c r="A9" s="9" t="s">
+        <v>108</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>109</v>
+      <c r="E9" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>115</v>
+      <c r="A10" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>109</v>
+      <c r="E10" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>116</v>
+      <c r="A12" s="9" t="s">
+        <v>110</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>109</v>
+      <c r="E12" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>117</v>
+      <c r="A13" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>103</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>109</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>118</v>
+      <c r="A14" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>109</v>
+      <c r="F14" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>119</v>
+      <c r="A16" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>109</v>
+      <c r="E16" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="A18" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>103</v>
+      </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="A19" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>103</v>
+      </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="A20" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>103</v>
+      </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="A21" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>103</v>
+      </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="A22" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>103</v>
+      </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
+      <c r="A24" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>103</v>
+      </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
+    <row r="25" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>103</v>
+      </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+    <row r="27" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A23:H23"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A4:H4"/>

</xml_diff>

<commit_message>
Izdesu mācība matriala piemerus
</commit_message>
<xml_diff>
--- a/LVT_TpM_TP_V_1_0_2_.xlsx
+++ b/LVT_TpM_TP_V_1_0_2_.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12900" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12900"/>
   </bookViews>
   <sheets>
     <sheet name="Apraksts" sheetId="1" r:id="rId1"/>
@@ -818,6 +818,9 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -838,9 +841,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1124,7 +1124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -1134,28 +1134,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1178,12 +1178,12 @@
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1275,8 +1275,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1287,10 +1287,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="18"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -1432,16 +1432,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -1470,16 +1470,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-    </row>
-    <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+    </row>
+    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>64</v>
       </c>
@@ -1532,14 +1532,14 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -1620,14 +1620,14 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -1708,16 +1708,16 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>84</v>
       </c>
@@ -1744,18 +1744,18 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-    </row>
-    <row r="18" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+    </row>
+    <row r="18" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>124</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>128</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>132</v>
       </c>
@@ -1886,14 +1886,14 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
@@ -2054,9 +2054,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19:F21"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,16 +2098,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -2132,14 +2132,14 @@
       <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -2186,14 +2186,14 @@
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -2262,16 +2262,16 @@
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-    </row>
-    <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>110</v>
       </c>
@@ -2293,7 +2293,7 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>111</v>
       </c>
@@ -2338,14 +2338,14 @@
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -2370,16 +2370,16 @@
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
@@ -2492,14 +2492,14 @@
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
@@ -2583,7 +2583,7 @@
       <c r="E27" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F27" s="19" t="s">
+      <c r="F27" s="12" t="s">
         <v>156</v>
       </c>
       <c r="G27" s="9" t="s">
@@ -2609,7 +2609,7 @@
       <c r="E28" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F28" s="19" t="s">
+      <c r="F28" s="12" t="s">
         <v>156</v>
       </c>
       <c r="G28" s="9" t="s">

</xml_diff>